<commit_message>
add result for sprot and treebank
</commit_message>
<xml_diff>
--- a/result/sprot/sprot.xlsx
+++ b/result/sprot/sprot.xlsx
@@ -5,19 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="194" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="194" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="overall" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="baseline" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="treejoin" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="binary_treejoin" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>树数</t>
   </si>
@@ -36,6 +37,9 @@
   <si>
     <t>prefix过滤后结果数</t>
   </si>
+  <si>
+    <t>平均前缀长度</t>
+  </si>
 </sst>
 </file>
 
@@ -44,7 +48,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -71,11 +75,6 @@
       <name val="Droid Sans Fallback"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Droid Sans Fallback"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -120,16 +119,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -152,8 +147,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -166,15 +161,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="n">
-        <v>56384</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>3829896</v>
+        <v>5512531</v>
       </c>
     </row>
   </sheetData>
@@ -195,8 +190,8 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -228,7 +223,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>12430424</v>
+        <v>9630</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>9.2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -236,7 +234,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>15324769</v>
+        <v>23708</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>9.4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -244,7 +245,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>19980884</v>
+        <v>46528</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>9.6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -252,7 +256,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>24624707</v>
+        <v>115900</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>9.9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -260,7 +267,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>30354228</v>
+        <v>226265</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>10.8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -268,7 +278,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>41898251</v>
+        <v>350893</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>11.4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -276,7 +289,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>57789548</v>
+        <v>508551</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>11.7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -284,7 +300,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>58973060</v>
+        <v>711554</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>12.7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -292,7 +311,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>93634630</v>
+        <v>1020818</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -300,7 +322,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>116157951</v>
+        <v>1498443</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>15.9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -308,7 +333,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>141602341</v>
+        <v>2217478</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>18.4</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -316,7 +344,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>169954664</v>
+        <v>3314531</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>22.8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -324,7 +355,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>203730247</v>
+        <v>5011873</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>29.7</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -332,7 +366,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>239306091</v>
+        <v>7654942</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>40.9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,7 +377,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>280539219</v>
+        <v>11811365</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>58.6</v>
       </c>
     </row>
   </sheetData>
@@ -359,10 +399,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -386,13 +426,22 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>55924</v>
+        <v>751</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2.29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -400,7 +449,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>55771</v>
+        <v>3600</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>3.89</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -408,7 +463,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>55587</v>
+        <v>11263</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>5.65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -416,7 +477,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>55303</v>
+        <v>21267</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>7.55</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -424,7 +491,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>54284</v>
+        <v>52878</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>9.58</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -432,7 +505,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>53552</v>
+        <v>94880</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>11.85</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -440,7 +519,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>53552</v>
+        <v>162303</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>14.29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -448,7 +533,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>52760</v>
+        <v>219410</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>16.81</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -456,7 +547,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>51792</v>
+        <v>317492</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>19.35</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -464,7 +561,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>50749</v>
+        <v>438052</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>21.91</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -472,7 +575,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>49556</v>
+        <v>659126</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>24.48</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -480,7 +589,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>48161</v>
+        <v>982078</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>10.6</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>27.06</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -488,7 +603,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>46609</v>
+        <v>1523786</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>14.9</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>29.63</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -496,7 +617,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>45027</v>
+        <v>2323163</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>32.18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -504,7 +631,268 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>43431</v>
+        <v>3621980</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>34.74</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.5612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>752</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2.51</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>3581</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>4.15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>11138</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>5.93</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>20618</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>7.84</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>50495</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>86290</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>12.13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>148169</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>14.44</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>201341</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>16.81</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>294175</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>10.1</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>390232</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>12.6</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>562101</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>23.81</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>806513</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>19.8</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>26.15</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>1241998</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>1873677</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>30.87</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>2929126</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>42.8</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>33.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>